<commit_message>
Updated to reflect new ULN process
</commit_message>
<xml_diff>
--- a/Manifest_Template.xlsx
+++ b/Manifest_Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-315" yWindow="585" windowWidth="15300" windowHeight="8520" firstSheet="3" activeTab="3"/>
@@ -15,8 +15,8 @@
     <sheet name="Instructions" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Final_Manifest!$B$1:$J$90</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Pre_Manifest!$B$1:$J$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Final_Manifest!$B$1:$I$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Pre_Manifest!$B$1:$I$90</definedName>
     <definedName name="OLE_LINK1" localSheetId="4">Final_Manifest!#REF!</definedName>
     <definedName name="OLE_LINK1" localSheetId="3">Pre_Manifest!#REF!</definedName>
   </definedNames>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="360">
   <si>
     <t>RAHLI REDOUANE</t>
   </si>
@@ -1120,13 +1120,10 @@
     <t>PRINCE, DIANA</t>
   </si>
   <si>
-    <t>INTRA_THEATER_ULN</t>
-  </si>
-  <si>
-    <t>TO_THEATER_ULN</t>
-  </si>
-  <si>
     <t>AFSC_MOS</t>
+  </si>
+  <si>
+    <t>ULN</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1723,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1888,7 +1885,6 @@
     <xf numFmtId="0" fontId="32" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1911,12 +1907,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1990,7 +1988,7 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -2236,49 +2234,6 @@
               <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>INTRA_THEATER_ULN</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>:  The ULN assigned to the passenger for movement </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>*</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>within* </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>theater.  This column is filled by reception, staging, and onward movement (RSO) teams in theater.  This column may be empty for passengers who do not know their final destination within theater.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
             <a:t>AFSC_MOS</a:t>
           </a:r>
           <a:r>
@@ -2426,28 +2381,14 @@
               <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>TO_THEATER_ULN</a:t>
+            <a:t>ULN</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>:  The ULN assigned to the passenger for movement </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>*to*</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t> theater.  This column is provided to the CRC by a higher authority (HRC?).</a:t>
+            <a:t>:  The ULN assigned to the passenger for movement from the mobilization station to their duty location in theater.  </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -11353,7 +11294,7 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:R150"/>
+  <dimension ref="A1:Q150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
@@ -11362,93 +11303,89 @@
     <col min="1" max="1" width="4.88671875" style="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.109375" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.21875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="41" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="38" customWidth="1"/>
-    <col min="10" max="10" width="19" style="38" customWidth="1"/>
-    <col min="11" max="11" width="18" style="38" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" style="38" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" style="38" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="38"/>
+    <col min="4" max="4" width="10.33203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="38" customWidth="1"/>
+    <col min="9" max="9" width="19" style="38" customWidth="1"/>
+    <col min="10" max="10" width="18" style="38" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" style="38" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" style="38" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="44" customFormat="1" ht="63" customHeight="1">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:17" s="44" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="75" t="s">
         <v>358</v>
       </c>
-      <c r="E1" s="76" t="s">
-        <v>360</v>
-      </c>
-      <c r="F1" s="75" t="s">
+      <c r="E1" s="74" t="s">
         <v>333</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="F1" s="74" t="s">
         <v>334</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="G1" s="74" t="s">
         <v>335</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="H1" s="74" t="s">
         <v>336</v>
       </c>
-      <c r="J1" s="75" t="s">
+      <c r="I1" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="J1" s="73" t="s">
         <v>359</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="K1" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="L1" s="73" t="s">
         <v>344</v>
       </c>
+      <c r="M1" s="43"/>
       <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="B2" s="39"/>
-      <c r="G2" s="42"/>
-      <c r="J2" s="39"/>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1">
+      <c r="F2" s="42"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="B3" s="39"/>
-      <c r="G3" s="42"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1">
+      <c r="F3" s="42"/>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="B4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="43"/>
       <c r="K4" s="43"/>
       <c r="L4" s="43"/>
       <c r="M4" s="43"/>
       <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
+      <c r="O4" s="44"/>
       <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-    </row>
-    <row r="5" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="5" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B5" s="39"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
@@ -11456,90 +11393,86 @@
       <c r="O5" s="38"/>
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1">
       <c r="B6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="O6" s="46"/>
-    </row>
-    <row r="7" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I6" s="39"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B7" s="39"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="38"/>
       <c r="L7" s="38"/>
       <c r="M7" s="38"/>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1">
       <c r="B8" s="39"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="39"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
       <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
+      <c r="O9" s="46"/>
       <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-    </row>
-    <row r="10" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B10" s="39"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
       <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
       <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1">
       <c r="B11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="P11" s="46"/>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
+      <c r="I11" s="39"/>
+      <c r="O11" s="46"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1">
       <c r="B12" s="39"/>
-      <c r="J12" s="39"/>
-    </row>
-    <row r="13" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="1:17" s="46" customFormat="1" ht="15" customHeight="1">
       <c r="B13" s="39"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="G13" s="38"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
@@ -11547,226 +11480,219 @@
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-    </row>
-    <row r="14" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="14" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B14" s="39"/>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-    </row>
-    <row r="15" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B15" s="39"/>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="38"/>
       <c r="K15" s="38"/>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="B16" s="39"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="45"/>
-      <c r="J16" s="39"/>
-    </row>
-    <row r="17" spans="2:17" ht="15" customHeight="1">
+      <c r="F16" s="66"/>
+      <c r="G16" s="45"/>
+      <c r="I16" s="39"/>
+    </row>
+    <row r="17" spans="2:16" ht="15" customHeight="1">
       <c r="B17" s="39"/>
-      <c r="G17" s="42"/>
-      <c r="J17" s="39"/>
-    </row>
-    <row r="18" spans="2:17" ht="15" customHeight="1">
+      <c r="F17" s="42"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="2:16" ht="15" customHeight="1">
       <c r="B18" s="39"/>
-      <c r="J18" s="39"/>
-    </row>
-    <row r="19" spans="2:17" ht="15" customHeight="1">
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="2:16" ht="15" customHeight="1">
       <c r="B19" s="39"/>
-      <c r="J19" s="39"/>
-    </row>
-    <row r="20" spans="2:17" ht="15" customHeight="1">
+      <c r="I19" s="39"/>
+    </row>
+    <row r="20" spans="2:16" ht="15" customHeight="1">
       <c r="B20" s="39"/>
-      <c r="J20" s="39"/>
-    </row>
-    <row r="21" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I20" s="39"/>
+    </row>
+    <row r="21" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B21" s="39"/>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="38"/>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
       <c r="O21" s="38"/>
       <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-    </row>
-    <row r="22" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B22" s="39"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="38"/>
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
       <c r="O22" s="38"/>
       <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-    </row>
-    <row r="23" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B23" s="39"/>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+      <c r="G23" s="38"/>
       <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="38"/>
       <c r="K23" s="38"/>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
       <c r="O23" s="38"/>
       <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-    </row>
-    <row r="24" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B24" s="39"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="G24" s="38"/>
       <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="38"/>
       <c r="K24" s="38"/>
       <c r="L24" s="38"/>
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38"/>
       <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-    </row>
-    <row r="25" spans="2:17" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="2:16" ht="15" customHeight="1">
       <c r="B25" s="39"/>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="2:17" ht="15" customHeight="1">
+      <c r="I25" s="39"/>
+    </row>
+    <row r="26" spans="2:16" ht="15" customHeight="1">
       <c r="B26" s="39"/>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="2:17" ht="15" customHeight="1">
+      <c r="I26" s="39"/>
+    </row>
+    <row r="27" spans="2:16" ht="15" customHeight="1">
       <c r="B27" s="39"/>
-      <c r="G27" s="42"/>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="2:17" ht="15" customHeight="1">
+      <c r="F27" s="42"/>
+      <c r="I27" s="39"/>
+    </row>
+    <row r="28" spans="2:16" ht="15" customHeight="1">
       <c r="B28" s="39"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="45"/>
-      <c r="J28" s="39"/>
-    </row>
-    <row r="29" spans="2:17" ht="15" customHeight="1">
+      <c r="F28" s="66"/>
+      <c r="G28" s="45"/>
+      <c r="I28" s="39"/>
+    </row>
+    <row r="29" spans="2:16" ht="15" customHeight="1">
       <c r="B29" s="36"/>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="2:17" ht="15" customHeight="1">
+      <c r="I29" s="39"/>
+    </row>
+    <row r="30" spans="2:16" ht="15" customHeight="1">
       <c r="B30" s="39"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="45"/>
-      <c r="J30" s="39"/>
-    </row>
-    <row r="31" spans="2:17" ht="15" customHeight="1">
+      <c r="F30" s="66"/>
+      <c r="G30" s="45"/>
+      <c r="I30" s="39"/>
+    </row>
+    <row r="31" spans="2:16" ht="15" customHeight="1">
       <c r="B31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="Q31" s="46"/>
-    </row>
-    <row r="32" spans="2:17" ht="15" customHeight="1">
+      <c r="I31" s="39"/>
+      <c r="P31" s="46"/>
+    </row>
+    <row r="32" spans="2:16" ht="15" customHeight="1">
       <c r="B32" s="39"/>
-      <c r="J32" s="39"/>
-    </row>
-    <row r="33" spans="2:18" ht="15" customHeight="1">
+      <c r="I32" s="39"/>
+    </row>
+    <row r="33" spans="2:17" ht="15" customHeight="1">
       <c r="B33" s="39"/>
-      <c r="J33" s="39"/>
-    </row>
-    <row r="34" spans="2:18" ht="15" customHeight="1">
+      <c r="I33" s="39"/>
+    </row>
+    <row r="34" spans="2:17" ht="15" customHeight="1">
       <c r="B34" s="39"/>
-      <c r="J34" s="39"/>
-    </row>
-    <row r="35" spans="2:18" ht="15" customHeight="1">
+      <c r="I34" s="39"/>
+    </row>
+    <row r="35" spans="2:17" ht="15" customHeight="1">
       <c r="B35" s="39"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="45"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="2:18" ht="15" customHeight="1">
+      <c r="F35" s="66"/>
+      <c r="G35" s="45"/>
+      <c r="I35" s="39"/>
+    </row>
+    <row r="36" spans="2:17" ht="15" customHeight="1">
       <c r="B36" s="39"/>
-      <c r="J36" s="39"/>
-    </row>
-    <row r="37" spans="2:18" ht="15" customHeight="1">
+      <c r="I36" s="39"/>
+    </row>
+    <row r="37" spans="2:17" ht="15" customHeight="1">
       <c r="B37" s="39"/>
-      <c r="J37" s="39"/>
-    </row>
-    <row r="38" spans="2:18" ht="15" customHeight="1">
+      <c r="I37" s="39"/>
+    </row>
+    <row r="38" spans="2:17" ht="15" customHeight="1">
       <c r="B38" s="39"/>
-      <c r="G38" s="42"/>
-      <c r="J38" s="39"/>
-    </row>
-    <row r="39" spans="2:18" ht="15" customHeight="1">
+      <c r="F38" s="42"/>
+      <c r="I38" s="39"/>
+    </row>
+    <row r="39" spans="2:17" ht="15" customHeight="1">
       <c r="B39" s="39"/>
-      <c r="J39" s="39"/>
-    </row>
-    <row r="40" spans="2:18" ht="15" customHeight="1">
+      <c r="I39" s="39"/>
+    </row>
+    <row r="40" spans="2:17" ht="15" customHeight="1">
       <c r="B40" s="39"/>
-      <c r="J40" s="39"/>
-    </row>
-    <row r="41" spans="2:18" ht="15" customHeight="1">
+      <c r="I40" s="39"/>
+    </row>
+    <row r="41" spans="2:17" ht="15" customHeight="1">
       <c r="B41" s="39"/>
-      <c r="J41" s="39"/>
-    </row>
-    <row r="42" spans="2:18" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="I41" s="39"/>
+    </row>
+    <row r="42" spans="2:17" s="46" customFormat="1" ht="15" customHeight="1">
       <c r="B42" s="39"/>
       <c r="C42" s="41"/>
       <c r="D42" s="41"/>
       <c r="E42" s="41"/>
       <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="G42" s="38"/>
       <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="38"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
@@ -11774,264 +11700,254 @@
       <c r="O42" s="38"/>
       <c r="P42" s="38"/>
       <c r="Q42" s="38"/>
-      <c r="R42" s="38"/>
-    </row>
-    <row r="43" spans="2:18" ht="15" customHeight="1">
+    </row>
+    <row r="43" spans="2:17" ht="15" customHeight="1">
       <c r="B43" s="39"/>
-      <c r="H43" s="68"/>
-      <c r="J43" s="39"/>
-    </row>
-    <row r="44" spans="2:18" ht="15" customHeight="1">
+      <c r="G43" s="68"/>
+      <c r="I43" s="39"/>
+    </row>
+    <row r="44" spans="2:17" ht="15" customHeight="1">
       <c r="B44" s="39"/>
-      <c r="G44" s="42"/>
-      <c r="J44" s="39"/>
-    </row>
-    <row r="45" spans="2:18" ht="15" customHeight="1">
+      <c r="F44" s="42"/>
+      <c r="I44" s="39"/>
+    </row>
+    <row r="45" spans="2:17" ht="15" customHeight="1">
       <c r="B45" s="39"/>
-      <c r="J45" s="39"/>
-    </row>
-    <row r="46" spans="2:18" ht="15" customHeight="1">
+      <c r="I45" s="39"/>
+    </row>
+    <row r="46" spans="2:17" ht="15" customHeight="1">
       <c r="B46" s="39"/>
-      <c r="J46" s="39"/>
-    </row>
-    <row r="47" spans="2:18" ht="15" customHeight="1">
+      <c r="I46" s="39"/>
+    </row>
+    <row r="47" spans="2:17" ht="15" customHeight="1">
       <c r="B47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="R47" s="46"/>
-    </row>
-    <row r="48" spans="2:18" ht="15" customHeight="1">
+      <c r="I47" s="39"/>
+      <c r="Q47" s="46"/>
+    </row>
+    <row r="48" spans="2:17" ht="15" customHeight="1">
       <c r="B48" s="39"/>
-      <c r="H48" s="68"/>
-      <c r="J48" s="39"/>
-    </row>
-    <row r="49" spans="2:18" ht="15" customHeight="1">
+      <c r="G48" s="68"/>
+      <c r="I48" s="39"/>
+    </row>
+    <row r="49" spans="2:17" ht="15" customHeight="1">
       <c r="B49" s="39"/>
-      <c r="G49" s="42"/>
-      <c r="J49" s="39"/>
-    </row>
-    <row r="50" spans="2:18" ht="15" customHeight="1">
+      <c r="F49" s="42"/>
+      <c r="I49" s="39"/>
+    </row>
+    <row r="50" spans="2:17" ht="15" customHeight="1">
       <c r="B50" s="39"/>
-      <c r="H50" s="45"/>
-      <c r="J50" s="39"/>
-    </row>
-    <row r="51" spans="2:18" ht="15" customHeight="1">
+      <c r="G50" s="45"/>
+      <c r="I50" s="39"/>
+    </row>
+    <row r="51" spans="2:17" ht="15" customHeight="1">
       <c r="B51" s="39"/>
-      <c r="J51" s="39"/>
-    </row>
-    <row r="52" spans="2:18" ht="15" customHeight="1">
+      <c r="I51" s="39"/>
+    </row>
+    <row r="52" spans="2:17" ht="15" customHeight="1">
       <c r="B52" s="36"/>
-      <c r="J52" s="39"/>
-    </row>
-    <row r="53" spans="2:18" ht="15" customHeight="1">
+      <c r="I52" s="39"/>
+    </row>
+    <row r="53" spans="2:17" ht="15" customHeight="1">
       <c r="B53" s="39"/>
-      <c r="G53" s="42"/>
-      <c r="J53" s="39"/>
-    </row>
-    <row r="54" spans="2:18" ht="15" customHeight="1">
+      <c r="F53" s="42"/>
+      <c r="I53" s="39"/>
+    </row>
+    <row r="54" spans="2:17" ht="15" customHeight="1">
       <c r="B54" s="39"/>
-      <c r="J54" s="39"/>
-    </row>
-    <row r="55" spans="2:18" ht="15" customHeight="1">
+      <c r="I54" s="39"/>
+    </row>
+    <row r="55" spans="2:17" ht="15" customHeight="1">
       <c r="B55" s="39"/>
-      <c r="G55" s="42"/>
-      <c r="J55" s="39"/>
+      <c r="F55" s="42"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="47"/>
       <c r="K55" s="47"/>
       <c r="L55" s="47"/>
       <c r="M55" s="47"/>
       <c r="N55" s="47"/>
       <c r="O55" s="47"/>
-      <c r="P55" s="47"/>
+      <c r="P55" s="40"/>
       <c r="Q55" s="40"/>
-      <c r="R55" s="40"/>
-    </row>
-    <row r="56" spans="2:18" ht="15" customHeight="1">
+    </row>
+    <row r="56" spans="2:17" ht="15" customHeight="1">
       <c r="B56" s="39"/>
-      <c r="G56" s="42"/>
-      <c r="J56" s="39"/>
-    </row>
-    <row r="57" spans="2:18" ht="15" customHeight="1">
+      <c r="F56" s="42"/>
+      <c r="I56" s="39"/>
+    </row>
+    <row r="57" spans="2:17" ht="15" customHeight="1">
       <c r="B57" s="36"/>
-      <c r="J57" s="39"/>
-    </row>
-    <row r="58" spans="2:18" ht="15" customHeight="1">
+      <c r="I57" s="39"/>
+    </row>
+    <row r="58" spans="2:17" ht="15" customHeight="1">
       <c r="B58" s="39"/>
-      <c r="H58" s="68"/>
-      <c r="J58" s="39"/>
-    </row>
-    <row r="59" spans="2:18" ht="15" customHeight="1">
+      <c r="G58" s="68"/>
+      <c r="I58" s="39"/>
+    </row>
+    <row r="59" spans="2:17" ht="15" customHeight="1">
       <c r="B59" s="39"/>
-      <c r="H59" s="45"/>
-      <c r="J59" s="39"/>
-    </row>
-    <row r="60" spans="2:18" ht="15" customHeight="1">
+      <c r="G59" s="45"/>
+      <c r="I59" s="39"/>
+    </row>
+    <row r="60" spans="2:17" ht="15" customHeight="1">
       <c r="B60" s="39"/>
-      <c r="J60" s="39"/>
-    </row>
-    <row r="61" spans="2:18" ht="15" customHeight="1">
+      <c r="I60" s="39"/>
+    </row>
+    <row r="61" spans="2:17" ht="15" customHeight="1">
       <c r="B61" s="39"/>
-      <c r="J61" s="39"/>
-    </row>
-    <row r="62" spans="2:18" ht="15" customHeight="1">
-      <c r="J62" s="39"/>
-    </row>
-    <row r="63" spans="2:18" ht="15" customHeight="1">
+      <c r="I61" s="39"/>
+    </row>
+    <row r="62" spans="2:17" ht="15" customHeight="1">
+      <c r="I62" s="39"/>
+    </row>
+    <row r="63" spans="2:17" ht="15" customHeight="1">
       <c r="B63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="R63" s="46"/>
-    </row>
-    <row r="64" spans="2:18" ht="15" customHeight="1">
+      <c r="I63" s="39"/>
+      <c r="Q63" s="46"/>
+    </row>
+    <row r="64" spans="2:17" ht="15" customHeight="1">
       <c r="B64" s="39"/>
-      <c r="H64" s="45"/>
-      <c r="J64" s="39"/>
-    </row>
-    <row r="65" spans="2:17" ht="15" customHeight="1">
+      <c r="G64" s="45"/>
+      <c r="I64" s="39"/>
+    </row>
+    <row r="65" spans="2:16" ht="15" customHeight="1">
       <c r="B65" s="39"/>
-      <c r="J65" s="39"/>
-    </row>
-    <row r="66" spans="2:17" ht="15" customHeight="1">
+      <c r="I65" s="39"/>
+    </row>
+    <row r="66" spans="2:16" ht="15" customHeight="1">
       <c r="B66" s="39"/>
-      <c r="J66" s="39"/>
-    </row>
-    <row r="67" spans="2:17" ht="15" customHeight="1">
+      <c r="I66" s="39"/>
+    </row>
+    <row r="67" spans="2:16" ht="15" customHeight="1">
       <c r="B67" s="39"/>
-      <c r="J67" s="39"/>
-    </row>
-    <row r="68" spans="2:17" ht="15" customHeight="1">
+      <c r="I67" s="39"/>
+    </row>
+    <row r="68" spans="2:16" ht="15" customHeight="1">
       <c r="B68" s="39"/>
-      <c r="J68" s="39"/>
-    </row>
-    <row r="69" spans="2:17" ht="15" customHeight="1">
+      <c r="I68" s="39"/>
+    </row>
+    <row r="69" spans="2:16" ht="15" customHeight="1">
       <c r="B69" s="39"/>
-      <c r="G69" s="42"/>
-      <c r="J69" s="39"/>
-    </row>
-    <row r="70" spans="2:17" ht="15" customHeight="1">
+      <c r="F69" s="42"/>
+      <c r="I69" s="39"/>
+    </row>
+    <row r="70" spans="2:16" ht="15" customHeight="1">
       <c r="B70" s="39"/>
-      <c r="J70" s="39"/>
-    </row>
-    <row r="71" spans="2:17" ht="15" customHeight="1">
+      <c r="I70" s="39"/>
+    </row>
+    <row r="71" spans="2:16" ht="15" customHeight="1">
       <c r="B71" s="39"/>
-      <c r="G71" s="67"/>
-      <c r="H71" s="45"/>
-      <c r="J71" s="39"/>
-    </row>
-    <row r="72" spans="2:17" ht="15" customHeight="1">
+      <c r="F71" s="67"/>
+      <c r="G71" s="45"/>
+      <c r="I71" s="39"/>
+    </row>
+    <row r="72" spans="2:16" ht="15" customHeight="1">
       <c r="B72" s="39"/>
-      <c r="G72" s="42"/>
-      <c r="J72" s="39"/>
-    </row>
-    <row r="73" spans="2:17" ht="15" customHeight="1">
+      <c r="F72" s="42"/>
+      <c r="I72" s="39"/>
+    </row>
+    <row r="73" spans="2:16" ht="15" customHeight="1">
       <c r="B73" s="39"/>
-      <c r="J73" s="39"/>
-    </row>
-    <row r="74" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I73" s="39"/>
+    </row>
+    <row r="74" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B74" s="35"/>
       <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="53"/>
-      <c r="F74" s="61"/>
-      <c r="G74" s="51"/>
-      <c r="H74" s="58"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="35"/>
+      <c r="D74" s="53"/>
+      <c r="E74" s="61"/>
+      <c r="F74" s="51"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="38"/>
       <c r="K74" s="38"/>
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
       <c r="N74" s="38"/>
       <c r="O74" s="38"/>
       <c r="P74" s="38"/>
-      <c r="Q74" s="38"/>
-    </row>
-    <row r="75" spans="2:17" ht="15" customHeight="1">
+    </row>
+    <row r="75" spans="2:16" ht="15" customHeight="1">
       <c r="B75" s="35"/>
       <c r="C75" s="51"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="61"/>
-      <c r="G75" s="51"/>
-      <c r="H75" s="58"/>
-      <c r="J75" s="35"/>
-    </row>
-    <row r="76" spans="2:17" ht="15" customHeight="1">
+      <c r="D75" s="53"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="51"/>
+      <c r="G75" s="58"/>
+      <c r="I75" s="35"/>
+    </row>
+    <row r="76" spans="2:16" ht="15" customHeight="1">
       <c r="B76" s="35"/>
       <c r="C76" s="51"/>
       <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="61"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="64"/>
-      <c r="J76" s="35"/>
-    </row>
-    <row r="77" spans="2:17" ht="15" customHeight="1">
+      <c r="E76" s="61"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="64"/>
+      <c r="I76" s="35"/>
+    </row>
+    <row r="77" spans="2:16" ht="15" customHeight="1">
       <c r="B77" s="35"/>
       <c r="C77" s="51"/>
       <c r="D77" s="51"/>
-      <c r="E77" s="51"/>
-      <c r="F77" s="61"/>
-      <c r="G77" s="51"/>
-      <c r="H77" s="64"/>
-      <c r="J77" s="35"/>
-    </row>
-    <row r="78" spans="2:17" ht="15" customHeight="1">
+      <c r="E77" s="61"/>
+      <c r="F77" s="51"/>
+      <c r="G77" s="64"/>
+      <c r="I77" s="35"/>
+    </row>
+    <row r="78" spans="2:16" ht="15" customHeight="1">
       <c r="B78" s="35"/>
       <c r="C78" s="51"/>
       <c r="D78" s="51"/>
-      <c r="E78" s="51"/>
-      <c r="F78" s="61"/>
-      <c r="G78" s="51"/>
-      <c r="H78" s="64"/>
-      <c r="J78" s="35"/>
-    </row>
-    <row r="79" spans="2:17" ht="15" customHeight="1">
+      <c r="E78" s="61"/>
+      <c r="F78" s="51"/>
+      <c r="G78" s="64"/>
+      <c r="I78" s="35"/>
+    </row>
+    <row r="79" spans="2:16" ht="15" customHeight="1">
       <c r="B79" s="35"/>
       <c r="C79" s="51"/>
       <c r="D79" s="51"/>
-      <c r="E79" s="51"/>
-      <c r="F79" s="61"/>
-      <c r="G79" s="51"/>
-      <c r="H79" s="64"/>
-      <c r="J79" s="35"/>
-    </row>
-    <row r="80" spans="2:17" ht="15" customHeight="1">
+      <c r="E79" s="61"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="64"/>
+      <c r="I79" s="35"/>
+    </row>
+    <row r="80" spans="2:16" ht="15" customHeight="1">
       <c r="B80" s="35"/>
       <c r="C80" s="51"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="53"/>
-      <c r="F80" s="61"/>
-      <c r="G80" s="51"/>
-      <c r="H80" s="58"/>
-      <c r="J80" s="35"/>
-    </row>
-    <row r="81" spans="2:18" ht="15" customHeight="1">
+      <c r="D80" s="53"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="51"/>
+      <c r="G80" s="58"/>
+      <c r="I80" s="35"/>
+    </row>
+    <row r="81" spans="2:17" ht="15" customHeight="1">
       <c r="B81" s="35"/>
       <c r="C81" s="51"/>
       <c r="D81" s="51"/>
-      <c r="E81" s="51"/>
-      <c r="F81" s="61"/>
-      <c r="G81" s="51"/>
-      <c r="H81" s="64"/>
-      <c r="J81" s="35"/>
-    </row>
-    <row r="82" spans="2:18" ht="15" customHeight="1">
+      <c r="E81" s="61"/>
+      <c r="F81" s="51"/>
+      <c r="G81" s="64"/>
+      <c r="I81" s="35"/>
+    </row>
+    <row r="82" spans="2:17" ht="15" customHeight="1">
       <c r="B82" s="35"/>
       <c r="C82" s="51"/>
       <c r="D82" s="51"/>
-      <c r="E82" s="51"/>
-      <c r="F82" s="61"/>
-      <c r="G82" s="51"/>
-      <c r="H82" s="64"/>
-      <c r="J82" s="6"/>
-    </row>
-    <row r="83" spans="2:18" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="E82" s="61"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="64"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B83" s="35"/>
       <c r="C83" s="51"/>
       <c r="D83" s="51"/>
-      <c r="E83" s="51"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="51"/>
-      <c r="H83" s="63"/>
-      <c r="I83" s="38"/>
-      <c r="J83" s="35"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="51"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="35"/>
+      <c r="J83" s="38"/>
       <c r="K83" s="38"/>
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>
@@ -12039,310 +11955,293 @@
       <c r="O83" s="38"/>
       <c r="P83" s="38"/>
       <c r="Q83" s="38"/>
-      <c r="R83" s="38"/>
-    </row>
-    <row r="84" spans="2:18" ht="15" customHeight="1">
+    </row>
+    <row r="84" spans="2:17" ht="15" customHeight="1">
       <c r="B84" s="35"/>
       <c r="C84" s="51"/>
       <c r="D84" s="51"/>
-      <c r="E84" s="51"/>
-      <c r="F84" s="61"/>
-      <c r="G84" s="51"/>
-      <c r="H84" s="63"/>
-      <c r="J84" s="35"/>
-    </row>
-    <row r="85" spans="2:18" ht="15" customHeight="1">
+      <c r="E84" s="61"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="63"/>
+      <c r="I84" s="35"/>
+    </row>
+    <row r="85" spans="2:17" ht="15" customHeight="1">
       <c r="B85" s="6"/>
       <c r="C85" s="51"/>
-      <c r="D85" s="51"/>
-      <c r="E85" s="53"/>
-      <c r="F85" s="61"/>
-      <c r="G85" s="51"/>
-      <c r="H85" s="58"/>
-      <c r="J85" s="35"/>
-    </row>
-    <row r="86" spans="2:18" ht="15" customHeight="1">
+      <c r="D85" s="53"/>
+      <c r="E85" s="61"/>
+      <c r="F85" s="51"/>
+      <c r="G85" s="58"/>
+      <c r="I85" s="35"/>
+    </row>
+    <row r="86" spans="2:17" ht="15" customHeight="1">
       <c r="B86" s="6"/>
       <c r="C86" s="51"/>
       <c r="D86" s="51"/>
-      <c r="E86" s="51"/>
-      <c r="F86" s="61"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="58"/>
-      <c r="J86" s="35"/>
-    </row>
-    <row r="87" spans="2:18" ht="15" customHeight="1">
+      <c r="E86" s="61"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="58"/>
+      <c r="I86" s="35"/>
+    </row>
+    <row r="87" spans="2:17" ht="15" customHeight="1">
       <c r="B87" s="35"/>
       <c r="C87" s="51"/>
       <c r="D87" s="51"/>
-      <c r="E87" s="51"/>
-      <c r="F87" s="50"/>
-      <c r="G87" s="51"/>
-      <c r="H87" s="59"/>
-      <c r="J87" s="35"/>
-    </row>
-    <row r="88" spans="2:18" ht="15" customHeight="1">
+      <c r="E87" s="50"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="59"/>
+      <c r="I87" s="35"/>
+    </row>
+    <row r="88" spans="2:17" ht="15" customHeight="1">
       <c r="B88" s="6"/>
       <c r="C88" s="51"/>
-      <c r="D88" s="51"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="61"/>
-      <c r="G88" s="51"/>
-      <c r="H88" s="59"/>
-      <c r="J88" s="35"/>
-    </row>
-    <row r="89" spans="2:18" ht="15" customHeight="1">
+      <c r="D88" s="53"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="51"/>
+      <c r="G88" s="59"/>
+      <c r="I88" s="35"/>
+    </row>
+    <row r="89" spans="2:17" ht="15" customHeight="1">
       <c r="B89" s="7"/>
       <c r="C89" s="54"/>
-      <c r="D89" s="54"/>
-      <c r="E89" s="62"/>
-      <c r="F89" s="50"/>
-      <c r="G89" s="61"/>
-      <c r="H89" s="65"/>
-      <c r="J89" s="65"/>
-    </row>
-    <row r="90" spans="2:18" ht="15" customHeight="1">
+      <c r="D89" s="62"/>
+      <c r="E89" s="50"/>
+      <c r="F89" s="61"/>
+      <c r="G89" s="65"/>
+      <c r="I89" s="65"/>
+    </row>
+    <row r="90" spans="2:17" ht="15" customHeight="1">
       <c r="B90" s="52"/>
       <c r="C90" s="48"/>
-      <c r="D90" s="48"/>
-      <c r="E90" s="49"/>
-      <c r="F90" s="55"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="52"/>
-      <c r="J90" s="52"/>
-    </row>
-    <row r="91" spans="2:18" ht="15" customHeight="1">
+      <c r="D90" s="49"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="56"/>
+      <c r="G90" s="52"/>
+      <c r="I90" s="52"/>
+    </row>
+    <row r="91" spans="2:17" ht="15" customHeight="1">
       <c r="B91" s="52"/>
       <c r="C91" s="48"/>
       <c r="D91" s="48"/>
-      <c r="E91" s="48"/>
-      <c r="F91" s="55"/>
-      <c r="G91" s="56"/>
-      <c r="H91" s="52"/>
-      <c r="J91" s="52"/>
-    </row>
-    <row r="92" spans="2:18" ht="15" customHeight="1">
+      <c r="E91" s="55"/>
+      <c r="F91" s="56"/>
+      <c r="G91" s="52"/>
+      <c r="I91" s="52"/>
+    </row>
+    <row r="92" spans="2:17" ht="15" customHeight="1">
       <c r="B92" s="52"/>
       <c r="C92" s="48"/>
       <c r="D92" s="48"/>
-      <c r="E92" s="48"/>
-      <c r="F92" s="55"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="52"/>
-      <c r="J92" s="52"/>
-    </row>
-    <row r="93" spans="2:18" ht="15" customHeight="1">
+      <c r="E92" s="55"/>
+      <c r="F92" s="56"/>
+      <c r="G92" s="52"/>
+      <c r="I92" s="52"/>
+    </row>
+    <row r="93" spans="2:17" ht="15" customHeight="1">
       <c r="B93" s="52"/>
       <c r="C93" s="48"/>
       <c r="D93" s="48"/>
-      <c r="E93" s="48"/>
-      <c r="F93" s="55"/>
-      <c r="G93" s="56"/>
-      <c r="H93" s="52"/>
-      <c r="J93" s="52"/>
-    </row>
-    <row r="94" spans="2:18" ht="15" customHeight="1">
+      <c r="E93" s="55"/>
+      <c r="F93" s="56"/>
+      <c r="G93" s="52"/>
+      <c r="I93" s="52"/>
+    </row>
+    <row r="94" spans="2:17" ht="15" customHeight="1">
       <c r="B94" s="52"/>
       <c r="C94" s="48"/>
       <c r="D94" s="48"/>
-      <c r="E94" s="48"/>
-      <c r="F94" s="55"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="52"/>
-      <c r="J94" s="52"/>
-    </row>
-    <row r="95" spans="2:18" ht="15" customHeight="1">
+      <c r="E94" s="55"/>
+      <c r="F94" s="56"/>
+      <c r="G94" s="52"/>
+      <c r="I94" s="52"/>
+    </row>
+    <row r="95" spans="2:17" ht="15" customHeight="1">
       <c r="B95" s="52"/>
       <c r="C95" s="48"/>
       <c r="D95" s="48"/>
-      <c r="E95" s="48"/>
-      <c r="F95" s="55"/>
-      <c r="G95" s="56"/>
-      <c r="H95" s="52"/>
-      <c r="J95" s="52"/>
-    </row>
-    <row r="96" spans="2:18" ht="15" customHeight="1">
+      <c r="E95" s="55"/>
+      <c r="F95" s="56"/>
+      <c r="G95" s="52"/>
+      <c r="I95" s="52"/>
+    </row>
+    <row r="96" spans="2:17" ht="15" customHeight="1">
       <c r="B96" s="52"/>
       <c r="C96" s="48"/>
       <c r="D96" s="48"/>
-      <c r="E96" s="48"/>
-      <c r="F96" s="55"/>
-      <c r="G96" s="56"/>
-      <c r="H96" s="52"/>
-      <c r="J96" s="52"/>
-    </row>
-    <row r="97" spans="2:10" ht="15" customHeight="1">
+      <c r="E96" s="55"/>
+      <c r="F96" s="56"/>
+      <c r="G96" s="52"/>
+      <c r="I96" s="52"/>
+    </row>
+    <row r="97" spans="2:9" ht="15" customHeight="1">
       <c r="B97" s="52"/>
       <c r="C97" s="48"/>
       <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="55"/>
-      <c r="G97" s="56"/>
-      <c r="H97" s="60"/>
-      <c r="J97" s="52"/>
-    </row>
-    <row r="98" spans="2:10" ht="15" customHeight="1">
+      <c r="E97" s="55"/>
+      <c r="F97" s="56"/>
+      <c r="G97" s="60"/>
+      <c r="I97" s="52"/>
+    </row>
+    <row r="98" spans="2:9" ht="15" customHeight="1">
       <c r="B98" s="52"/>
       <c r="C98" s="48"/>
       <c r="D98" s="48"/>
-      <c r="E98" s="48"/>
-      <c r="F98" s="55"/>
-      <c r="G98" s="57"/>
-      <c r="H98" s="60"/>
-      <c r="J98" s="52"/>
-    </row>
-    <row r="99" spans="2:10" ht="15" customHeight="1">
+      <c r="E98" s="55"/>
+      <c r="F98" s="57"/>
+      <c r="G98" s="60"/>
+      <c r="I98" s="52"/>
+    </row>
+    <row r="99" spans="2:9" ht="15" customHeight="1">
       <c r="B99" s="39"/>
-      <c r="G99" s="42"/>
-      <c r="H99" s="39"/>
-    </row>
-    <row r="100" spans="2:10" ht="15" customHeight="1">
+      <c r="F99" s="42"/>
+      <c r="G99" s="39"/>
+    </row>
+    <row r="100" spans="2:9" ht="15" customHeight="1">
       <c r="B100" s="39"/>
-      <c r="H100" s="39"/>
-    </row>
-    <row r="101" spans="2:10" ht="15" customHeight="1">
+      <c r="G100" s="39"/>
+    </row>
+    <row r="101" spans="2:9" ht="15" customHeight="1">
       <c r="B101" s="39"/>
-      <c r="H101" s="39"/>
-    </row>
-    <row r="102" spans="2:10" ht="15" customHeight="1">
+      <c r="G101" s="39"/>
+    </row>
+    <row r="102" spans="2:9" ht="15" customHeight="1">
       <c r="B102" s="39"/>
-      <c r="H102" s="39"/>
-      <c r="I102" s="45"/>
-    </row>
-    <row r="103" spans="2:10" ht="15" customHeight="1">
+      <c r="G102" s="39"/>
+      <c r="H102" s="45"/>
+    </row>
+    <row r="103" spans="2:9" ht="15" customHeight="1">
       <c r="B103" s="39"/>
-      <c r="G103" s="42"/>
-      <c r="H103" s="39"/>
-    </row>
-    <row r="104" spans="2:10" ht="15" customHeight="1">
+      <c r="F103" s="42"/>
+      <c r="G103" s="39"/>
+    </row>
+    <row r="104" spans="2:9" ht="15" customHeight="1">
       <c r="B104" s="39"/>
-      <c r="H104" s="39"/>
-    </row>
-    <row r="105" spans="2:10" ht="15" customHeight="1">
+      <c r="G104" s="39"/>
+    </row>
+    <row r="105" spans="2:9" ht="15" customHeight="1">
       <c r="B105" s="39"/>
-      <c r="G105" s="42"/>
-      <c r="H105" s="39"/>
-    </row>
-    <row r="106" spans="2:10" ht="15" customHeight="1">
+      <c r="F105" s="42"/>
+      <c r="G105" s="39"/>
+    </row>
+    <row r="106" spans="2:9" ht="15" customHeight="1">
       <c r="B106" s="39"/>
-      <c r="G106" s="42"/>
-      <c r="H106" s="39"/>
-    </row>
-    <row r="107" spans="2:10" ht="15" customHeight="1">
+      <c r="F106" s="42"/>
+      <c r="G106" s="39"/>
+    </row>
+    <row r="107" spans="2:9" ht="15" customHeight="1">
       <c r="B107" s="39"/>
-      <c r="H107" s="39"/>
-    </row>
-    <row r="108" spans="2:10" ht="15" customHeight="1">
+      <c r="G107" s="39"/>
+    </row>
+    <row r="108" spans="2:9" ht="15" customHeight="1">
       <c r="B108" s="39"/>
-      <c r="H108" s="39"/>
-    </row>
-    <row r="109" spans="2:10" ht="15" customHeight="1">
+      <c r="G108" s="39"/>
+    </row>
+    <row r="109" spans="2:9" ht="15" customHeight="1">
       <c r="B109" s="39"/>
-      <c r="H109" s="39"/>
-    </row>
-    <row r="110" spans="2:10" ht="15" customHeight="1">
+      <c r="G109" s="39"/>
+    </row>
+    <row r="110" spans="2:9" ht="15" customHeight="1">
       <c r="B110" s="39"/>
-      <c r="H110" s="39"/>
-    </row>
-    <row r="111" spans="2:10" ht="15" customHeight="1">
+      <c r="G110" s="39"/>
+    </row>
+    <row r="111" spans="2:9" ht="15" customHeight="1">
       <c r="B111" s="39"/>
-      <c r="H111" s="39"/>
-    </row>
-    <row r="112" spans="2:10" ht="15" customHeight="1">
+      <c r="G111" s="39"/>
+    </row>
+    <row r="112" spans="2:9" ht="15" customHeight="1">
       <c r="B112" s="39"/>
-      <c r="H112" s="39"/>
-    </row>
-    <row r="113" spans="2:8" ht="15" customHeight="1">
+      <c r="G112" s="39"/>
+    </row>
+    <row r="113" spans="2:7" ht="15" customHeight="1">
       <c r="B113" s="39"/>
-      <c r="H113" s="39"/>
-    </row>
-    <row r="114" spans="2:8" ht="15" customHeight="1">
+      <c r="G113" s="39"/>
+    </row>
+    <row r="114" spans="2:7" ht="15" customHeight="1">
       <c r="B114" s="39"/>
-      <c r="H114" s="39"/>
-    </row>
-    <row r="115" spans="2:8" ht="15" customHeight="1">
+      <c r="G114" s="39"/>
+    </row>
+    <row r="115" spans="2:7" ht="15" customHeight="1">
       <c r="B115" s="39"/>
-      <c r="H115" s="39"/>
-    </row>
-    <row r="116" spans="2:8" ht="15" customHeight="1">
+      <c r="G115" s="39"/>
+    </row>
+    <row r="116" spans="2:7" ht="15" customHeight="1">
       <c r="B116" s="39"/>
-      <c r="H116" s="39"/>
-    </row>
-    <row r="117" spans="2:8" ht="15" customHeight="1">
+      <c r="G116" s="39"/>
+    </row>
+    <row r="117" spans="2:7" ht="15" customHeight="1">
       <c r="B117" s="39"/>
-      <c r="G117" s="42"/>
-      <c r="H117" s="39"/>
-    </row>
-    <row r="118" spans="2:8" ht="15" customHeight="1">
+      <c r="F117" s="42"/>
+      <c r="G117" s="39"/>
+    </row>
+    <row r="118" spans="2:7" ht="15" customHeight="1">
       <c r="B118" s="39"/>
-      <c r="H118" s="39"/>
-    </row>
-    <row r="119" spans="2:8" ht="15" customHeight="1">
+      <c r="G118" s="39"/>
+    </row>
+    <row r="119" spans="2:7" ht="15" customHeight="1">
       <c r="B119" s="39"/>
-      <c r="G119" s="42"/>
-      <c r="H119" s="39"/>
-    </row>
-    <row r="120" spans="2:8" ht="15" customHeight="1">
+      <c r="F119" s="42"/>
+      <c r="G119" s="39"/>
+    </row>
+    <row r="120" spans="2:7" ht="15" customHeight="1">
       <c r="B120" s="39"/>
-      <c r="H120" s="39"/>
-    </row>
-    <row r="121" spans="2:8" ht="15" customHeight="1">
+      <c r="G120" s="39"/>
+    </row>
+    <row r="121" spans="2:7" ht="15" customHeight="1">
       <c r="B121" s="39"/>
-      <c r="G121" s="42"/>
-      <c r="H121" s="39"/>
-    </row>
-    <row r="122" spans="2:8" ht="15" customHeight="1">
+      <c r="F121" s="42"/>
+      <c r="G121" s="39"/>
+    </row>
+    <row r="122" spans="2:7" ht="15" customHeight="1">
       <c r="B122" s="39"/>
-      <c r="H122" s="39"/>
-    </row>
-    <row r="123" spans="2:8" ht="15" customHeight="1">
+      <c r="G122" s="39"/>
+    </row>
+    <row r="123" spans="2:7" ht="15" customHeight="1">
       <c r="B123" s="39"/>
-      <c r="G123" s="42"/>
-      <c r="H123" s="39"/>
-    </row>
-    <row r="124" spans="2:8" ht="15" customHeight="1">
+      <c r="F123" s="42"/>
+      <c r="G123" s="39"/>
+    </row>
+    <row r="124" spans="2:7" ht="15" customHeight="1">
       <c r="B124" s="39"/>
-      <c r="H124" s="39"/>
-    </row>
-    <row r="125" spans="2:8" ht="15" customHeight="1">
+      <c r="G124" s="39"/>
+    </row>
+    <row r="125" spans="2:7" ht="15" customHeight="1">
       <c r="B125" s="39"/>
-      <c r="H125" s="39"/>
-    </row>
-    <row r="126" spans="2:8" ht="15" customHeight="1">
+      <c r="G125" s="39"/>
+    </row>
+    <row r="126" spans="2:7" ht="15" customHeight="1">
       <c r="B126" s="36"/>
       <c r="C126" s="37"/>
       <c r="D126" s="37"/>
-      <c r="E126" s="37"/>
-      <c r="H126" s="36"/>
-    </row>
-    <row r="127" spans="2:8" ht="15" customHeight="1">
+      <c r="G126" s="36"/>
+    </row>
+    <row r="127" spans="2:7" ht="15" customHeight="1">
       <c r="B127" s="39"/>
-      <c r="G127" s="42"/>
-      <c r="H127" s="39"/>
-    </row>
-    <row r="143" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F143" s="51"/>
-    </row>
-    <row r="144" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F144" s="51"/>
-    </row>
-    <row r="145" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F145" s="51"/>
-    </row>
-    <row r="146" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F146" s="51"/>
-    </row>
-    <row r="147" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F147" s="51"/>
-    </row>
-    <row r="148" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F148" s="51"/>
-    </row>
-    <row r="149" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F149" s="51"/>
-    </row>
-    <row r="150" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F150" s="51"/>
+      <c r="F127" s="42"/>
+      <c r="G127" s="39"/>
+    </row>
+    <row r="143" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E143" s="51"/>
+    </row>
+    <row r="144" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E144" s="51"/>
+    </row>
+    <row r="145" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E145" s="51"/>
+    </row>
+    <row r="146" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E146" s="51"/>
+    </row>
+    <row r="147" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E147" s="51"/>
+    </row>
+    <row r="148" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E148" s="51"/>
+    </row>
+    <row r="149" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E149" s="51"/>
+    </row>
+    <row r="150" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E150" s="51"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -12361,102 +12260,100 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:R150"/>
+  <dimension ref="A1:Q150"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J2" sqref="J1:J1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4.88671875" style="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.109375" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.21875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="41" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="38" customWidth="1"/>
-    <col min="10" max="10" width="19" style="38" customWidth="1"/>
-    <col min="11" max="11" width="18" style="38" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" style="38" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" style="38" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="38"/>
+    <col min="4" max="4" width="10.33203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="38" customWidth="1"/>
+    <col min="9" max="9" width="19" style="38" customWidth="1"/>
+    <col min="10" max="10" width="18" style="38" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" style="38" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" style="38" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="44" customFormat="1" ht="63" customHeight="1">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:17" s="44" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="75" t="s">
         <v>358</v>
       </c>
-      <c r="E1" s="76" t="s">
-        <v>360</v>
-      </c>
-      <c r="F1" s="75" t="s">
+      <c r="E1" s="74" t="s">
         <v>333</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="F1" s="74" t="s">
         <v>334</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="G1" s="74" t="s">
         <v>335</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="H1" s="74" t="s">
         <v>336</v>
       </c>
-      <c r="J1" s="75" t="s">
+      <c r="I1" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="J1" s="73" t="s">
         <v>359</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="K1" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="L1" s="73" t="s">
         <v>344</v>
       </c>
+      <c r="M1" s="43"/>
       <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="B2" s="39"/>
-      <c r="G2" s="42"/>
-      <c r="J2" s="39"/>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1">
+      <c r="F2" s="42"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="B3" s="39"/>
-      <c r="G3" s="42"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1">
+      <c r="F3" s="42"/>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="B4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="43"/>
       <c r="K4" s="43"/>
       <c r="L4" s="43"/>
       <c r="M4" s="43"/>
       <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
+      <c r="O4" s="44"/>
       <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-    </row>
-    <row r="5" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="5" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B5" s="39"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
@@ -12464,90 +12361,86 @@
       <c r="O5" s="38"/>
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1">
       <c r="B6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="O6" s="46"/>
-    </row>
-    <row r="7" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I6" s="39"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B7" s="39"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="38"/>
       <c r="L7" s="38"/>
       <c r="M7" s="38"/>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1">
       <c r="B8" s="39"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="39"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
       <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
+      <c r="O9" s="46"/>
       <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-    </row>
-    <row r="10" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B10" s="39"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
       <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
       <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1">
       <c r="B11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="P11" s="46"/>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
+      <c r="I11" s="39"/>
+      <c r="O11" s="46"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1">
       <c r="B12" s="39"/>
-      <c r="J12" s="39"/>
-    </row>
-    <row r="13" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="1:17" s="46" customFormat="1" ht="15" customHeight="1">
       <c r="B13" s="39"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="G13" s="38"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
@@ -12555,226 +12448,219 @@
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-    </row>
-    <row r="14" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="14" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B14" s="39"/>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-    </row>
-    <row r="15" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B15" s="39"/>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="38"/>
       <c r="K15" s="38"/>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="B16" s="39"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="45"/>
-      <c r="J16" s="39"/>
-    </row>
-    <row r="17" spans="2:17" ht="15" customHeight="1">
+      <c r="F16" s="66"/>
+      <c r="G16" s="45"/>
+      <c r="I16" s="39"/>
+    </row>
+    <row r="17" spans="2:16" ht="15" customHeight="1">
       <c r="B17" s="39"/>
-      <c r="G17" s="42"/>
-      <c r="J17" s="39"/>
-    </row>
-    <row r="18" spans="2:17" ht="15" customHeight="1">
+      <c r="F17" s="42"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="2:16" ht="15" customHeight="1">
       <c r="B18" s="39"/>
-      <c r="J18" s="39"/>
-    </row>
-    <row r="19" spans="2:17" ht="15" customHeight="1">
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="2:16" ht="15" customHeight="1">
       <c r="B19" s="39"/>
-      <c r="J19" s="39"/>
-    </row>
-    <row r="20" spans="2:17" ht="15" customHeight="1">
+      <c r="I19" s="39"/>
+    </row>
+    <row r="20" spans="2:16" ht="15" customHeight="1">
       <c r="B20" s="39"/>
-      <c r="J20" s="39"/>
-    </row>
-    <row r="21" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I20" s="39"/>
+    </row>
+    <row r="21" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B21" s="39"/>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="38"/>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
       <c r="O21" s="38"/>
       <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-    </row>
-    <row r="22" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B22" s="39"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="38"/>
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
       <c r="O22" s="38"/>
       <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-    </row>
-    <row r="23" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B23" s="39"/>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+      <c r="G23" s="38"/>
       <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="38"/>
       <c r="K23" s="38"/>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
       <c r="O23" s="38"/>
       <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-    </row>
-    <row r="24" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B24" s="39"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="G24" s="38"/>
       <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="38"/>
       <c r="K24" s="38"/>
       <c r="L24" s="38"/>
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38"/>
       <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-    </row>
-    <row r="25" spans="2:17" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="2:16" ht="15" customHeight="1">
       <c r="B25" s="39"/>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="2:17" ht="15" customHeight="1">
+      <c r="I25" s="39"/>
+    </row>
+    <row r="26" spans="2:16" ht="15" customHeight="1">
       <c r="B26" s="39"/>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="2:17" ht="15" customHeight="1">
+      <c r="I26" s="39"/>
+    </row>
+    <row r="27" spans="2:16" ht="15" customHeight="1">
       <c r="B27" s="39"/>
-      <c r="G27" s="42"/>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="2:17" ht="15" customHeight="1">
+      <c r="F27" s="42"/>
+      <c r="I27" s="39"/>
+    </row>
+    <row r="28" spans="2:16" ht="15" customHeight="1">
       <c r="B28" s="39"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="45"/>
-      <c r="J28" s="39"/>
-    </row>
-    <row r="29" spans="2:17" ht="15" customHeight="1">
+      <c r="F28" s="66"/>
+      <c r="G28" s="45"/>
+      <c r="I28" s="39"/>
+    </row>
+    <row r="29" spans="2:16" ht="15" customHeight="1">
       <c r="B29" s="36"/>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="2:17" ht="15" customHeight="1">
+      <c r="I29" s="39"/>
+    </row>
+    <row r="30" spans="2:16" ht="15" customHeight="1">
       <c r="B30" s="39"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="45"/>
-      <c r="J30" s="39"/>
-    </row>
-    <row r="31" spans="2:17" ht="15" customHeight="1">
+      <c r="F30" s="66"/>
+      <c r="G30" s="45"/>
+      <c r="I30" s="39"/>
+    </row>
+    <row r="31" spans="2:16" ht="15" customHeight="1">
       <c r="B31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="Q31" s="46"/>
-    </row>
-    <row r="32" spans="2:17" ht="15" customHeight="1">
+      <c r="I31" s="39"/>
+      <c r="P31" s="46"/>
+    </row>
+    <row r="32" spans="2:16" ht="15" customHeight="1">
       <c r="B32" s="39"/>
-      <c r="J32" s="39"/>
-    </row>
-    <row r="33" spans="2:18" ht="15" customHeight="1">
+      <c r="I32" s="39"/>
+    </row>
+    <row r="33" spans="2:17" ht="15" customHeight="1">
       <c r="B33" s="39"/>
-      <c r="J33" s="39"/>
-    </row>
-    <row r="34" spans="2:18" ht="15" customHeight="1">
+      <c r="I33" s="39"/>
+    </row>
+    <row r="34" spans="2:17" ht="15" customHeight="1">
       <c r="B34" s="39"/>
-      <c r="J34" s="39"/>
-    </row>
-    <row r="35" spans="2:18" ht="15" customHeight="1">
+      <c r="I34" s="39"/>
+    </row>
+    <row r="35" spans="2:17" ht="15" customHeight="1">
       <c r="B35" s="39"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="45"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="2:18" ht="15" customHeight="1">
+      <c r="F35" s="66"/>
+      <c r="G35" s="45"/>
+      <c r="I35" s="39"/>
+    </row>
+    <row r="36" spans="2:17" ht="15" customHeight="1">
       <c r="B36" s="39"/>
-      <c r="J36" s="39"/>
-    </row>
-    <row r="37" spans="2:18" ht="15" customHeight="1">
+      <c r="I36" s="39"/>
+    </row>
+    <row r="37" spans="2:17" ht="15" customHeight="1">
       <c r="B37" s="39"/>
-      <c r="J37" s="39"/>
-    </row>
-    <row r="38" spans="2:18" ht="15" customHeight="1">
+      <c r="I37" s="39"/>
+    </row>
+    <row r="38" spans="2:17" ht="15" customHeight="1">
       <c r="B38" s="39"/>
-      <c r="G38" s="42"/>
-      <c r="J38" s="39"/>
-    </row>
-    <row r="39" spans="2:18" ht="15" customHeight="1">
+      <c r="F38" s="42"/>
+      <c r="I38" s="39"/>
+    </row>
+    <row r="39" spans="2:17" ht="15" customHeight="1">
       <c r="B39" s="39"/>
-      <c r="J39" s="39"/>
-    </row>
-    <row r="40" spans="2:18" ht="15" customHeight="1">
+      <c r="I39" s="39"/>
+    </row>
+    <row r="40" spans="2:17" ht="15" customHeight="1">
       <c r="B40" s="39"/>
-      <c r="J40" s="39"/>
-    </row>
-    <row r="41" spans="2:18" ht="15" customHeight="1">
+      <c r="I40" s="39"/>
+    </row>
+    <row r="41" spans="2:17" ht="15" customHeight="1">
       <c r="B41" s="39"/>
-      <c r="J41" s="39"/>
-    </row>
-    <row r="42" spans="2:18" s="46" customFormat="1" ht="15" customHeight="1">
+      <c r="I41" s="39"/>
+    </row>
+    <row r="42" spans="2:17" s="46" customFormat="1" ht="15" customHeight="1">
       <c r="B42" s="39"/>
       <c r="C42" s="41"/>
       <c r="D42" s="41"/>
       <c r="E42" s="41"/>
       <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="G42" s="38"/>
       <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="38"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
@@ -12782,264 +12668,254 @@
       <c r="O42" s="38"/>
       <c r="P42" s="38"/>
       <c r="Q42" s="38"/>
-      <c r="R42" s="38"/>
-    </row>
-    <row r="43" spans="2:18" ht="15" customHeight="1">
+    </row>
+    <row r="43" spans="2:17" ht="15" customHeight="1">
       <c r="B43" s="39"/>
-      <c r="H43" s="68"/>
-      <c r="J43" s="39"/>
-    </row>
-    <row r="44" spans="2:18" ht="15" customHeight="1">
+      <c r="G43" s="68"/>
+      <c r="I43" s="39"/>
+    </row>
+    <row r="44" spans="2:17" ht="15" customHeight="1">
       <c r="B44" s="39"/>
-      <c r="G44" s="42"/>
-      <c r="J44" s="39"/>
-    </row>
-    <row r="45" spans="2:18" ht="15" customHeight="1">
+      <c r="F44" s="42"/>
+      <c r="I44" s="39"/>
+    </row>
+    <row r="45" spans="2:17" ht="15" customHeight="1">
       <c r="B45" s="39"/>
-      <c r="J45" s="39"/>
-    </row>
-    <row r="46" spans="2:18" ht="15" customHeight="1">
+      <c r="I45" s="39"/>
+    </row>
+    <row r="46" spans="2:17" ht="15" customHeight="1">
       <c r="B46" s="39"/>
-      <c r="J46" s="39"/>
-    </row>
-    <row r="47" spans="2:18" ht="15" customHeight="1">
+      <c r="I46" s="39"/>
+    </row>
+    <row r="47" spans="2:17" ht="15" customHeight="1">
       <c r="B47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="R47" s="46"/>
-    </row>
-    <row r="48" spans="2:18" ht="15" customHeight="1">
+      <c r="I47" s="39"/>
+      <c r="Q47" s="46"/>
+    </row>
+    <row r="48" spans="2:17" ht="15" customHeight="1">
       <c r="B48" s="39"/>
-      <c r="H48" s="68"/>
-      <c r="J48" s="39"/>
-    </row>
-    <row r="49" spans="2:18" ht="15" customHeight="1">
+      <c r="G48" s="68"/>
+      <c r="I48" s="39"/>
+    </row>
+    <row r="49" spans="2:17" ht="15" customHeight="1">
       <c r="B49" s="39"/>
-      <c r="G49" s="42"/>
-      <c r="J49" s="39"/>
-    </row>
-    <row r="50" spans="2:18" ht="15" customHeight="1">
+      <c r="F49" s="42"/>
+      <c r="I49" s="39"/>
+    </row>
+    <row r="50" spans="2:17" ht="15" customHeight="1">
       <c r="B50" s="39"/>
-      <c r="H50" s="45"/>
-      <c r="J50" s="39"/>
-    </row>
-    <row r="51" spans="2:18" ht="15" customHeight="1">
+      <c r="G50" s="45"/>
+      <c r="I50" s="39"/>
+    </row>
+    <row r="51" spans="2:17" ht="15" customHeight="1">
       <c r="B51" s="39"/>
-      <c r="J51" s="39"/>
-    </row>
-    <row r="52" spans="2:18" ht="15" customHeight="1">
+      <c r="I51" s="39"/>
+    </row>
+    <row r="52" spans="2:17" ht="15" customHeight="1">
       <c r="B52" s="36"/>
-      <c r="J52" s="39"/>
-    </row>
-    <row r="53" spans="2:18" ht="15" customHeight="1">
+      <c r="I52" s="39"/>
+    </row>
+    <row r="53" spans="2:17" ht="15" customHeight="1">
       <c r="B53" s="39"/>
-      <c r="G53" s="42"/>
-      <c r="J53" s="39"/>
-    </row>
-    <row r="54" spans="2:18" ht="15" customHeight="1">
+      <c r="F53" s="42"/>
+      <c r="I53" s="39"/>
+    </row>
+    <row r="54" spans="2:17" ht="15" customHeight="1">
       <c r="B54" s="39"/>
-      <c r="J54" s="39"/>
-    </row>
-    <row r="55" spans="2:18" ht="15" customHeight="1">
+      <c r="I54" s="39"/>
+    </row>
+    <row r="55" spans="2:17" ht="15" customHeight="1">
       <c r="B55" s="39"/>
-      <c r="G55" s="42"/>
-      <c r="J55" s="39"/>
+      <c r="F55" s="42"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="47"/>
       <c r="K55" s="47"/>
       <c r="L55" s="47"/>
       <c r="M55" s="47"/>
       <c r="N55" s="47"/>
       <c r="O55" s="47"/>
-      <c r="P55" s="47"/>
+      <c r="P55" s="40"/>
       <c r="Q55" s="40"/>
-      <c r="R55" s="40"/>
-    </row>
-    <row r="56" spans="2:18" ht="15" customHeight="1">
+    </row>
+    <row r="56" spans="2:17" ht="15" customHeight="1">
       <c r="B56" s="39"/>
-      <c r="G56" s="42"/>
-      <c r="J56" s="39"/>
-    </row>
-    <row r="57" spans="2:18" ht="15" customHeight="1">
+      <c r="F56" s="42"/>
+      <c r="I56" s="39"/>
+    </row>
+    <row r="57" spans="2:17" ht="15" customHeight="1">
       <c r="B57" s="36"/>
-      <c r="J57" s="39"/>
-    </row>
-    <row r="58" spans="2:18" ht="15" customHeight="1">
+      <c r="I57" s="39"/>
+    </row>
+    <row r="58" spans="2:17" ht="15" customHeight="1">
       <c r="B58" s="39"/>
-      <c r="H58" s="68"/>
-      <c r="J58" s="39"/>
-    </row>
-    <row r="59" spans="2:18" ht="15" customHeight="1">
+      <c r="G58" s="68"/>
+      <c r="I58" s="39"/>
+    </row>
+    <row r="59" spans="2:17" ht="15" customHeight="1">
       <c r="B59" s="39"/>
-      <c r="H59" s="45"/>
-      <c r="J59" s="39"/>
-    </row>
-    <row r="60" spans="2:18" ht="15" customHeight="1">
+      <c r="G59" s="45"/>
+      <c r="I59" s="39"/>
+    </row>
+    <row r="60" spans="2:17" ht="15" customHeight="1">
       <c r="B60" s="39"/>
-      <c r="J60" s="39"/>
-    </row>
-    <row r="61" spans="2:18" ht="15" customHeight="1">
+      <c r="I60" s="39"/>
+    </row>
+    <row r="61" spans="2:17" ht="15" customHeight="1">
       <c r="B61" s="39"/>
-      <c r="J61" s="39"/>
-    </row>
-    <row r="62" spans="2:18" ht="15" customHeight="1">
-      <c r="J62" s="39"/>
-    </row>
-    <row r="63" spans="2:18" ht="15" customHeight="1">
+      <c r="I61" s="39"/>
+    </row>
+    <row r="62" spans="2:17" ht="15" customHeight="1">
+      <c r="I62" s="39"/>
+    </row>
+    <row r="63" spans="2:17" ht="15" customHeight="1">
       <c r="B63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="R63" s="46"/>
-    </row>
-    <row r="64" spans="2:18" ht="15" customHeight="1">
+      <c r="I63" s="39"/>
+      <c r="Q63" s="46"/>
+    </row>
+    <row r="64" spans="2:17" ht="15" customHeight="1">
       <c r="B64" s="39"/>
-      <c r="H64" s="45"/>
-      <c r="J64" s="39"/>
-    </row>
-    <row r="65" spans="2:17" ht="15" customHeight="1">
+      <c r="G64" s="45"/>
+      <c r="I64" s="39"/>
+    </row>
+    <row r="65" spans="2:16" ht="15" customHeight="1">
       <c r="B65" s="39"/>
-      <c r="J65" s="39"/>
-    </row>
-    <row r="66" spans="2:17" ht="15" customHeight="1">
+      <c r="I65" s="39"/>
+    </row>
+    <row r="66" spans="2:16" ht="15" customHeight="1">
       <c r="B66" s="39"/>
-      <c r="J66" s="39"/>
-    </row>
-    <row r="67" spans="2:17" ht="15" customHeight="1">
+      <c r="I66" s="39"/>
+    </row>
+    <row r="67" spans="2:16" ht="15" customHeight="1">
       <c r="B67" s="39"/>
-      <c r="J67" s="39"/>
-    </row>
-    <row r="68" spans="2:17" ht="15" customHeight="1">
+      <c r="I67" s="39"/>
+    </row>
+    <row r="68" spans="2:16" ht="15" customHeight="1">
       <c r="B68" s="39"/>
-      <c r="J68" s="39"/>
-    </row>
-    <row r="69" spans="2:17" ht="15" customHeight="1">
+      <c r="I68" s="39"/>
+    </row>
+    <row r="69" spans="2:16" ht="15" customHeight="1">
       <c r="B69" s="39"/>
-      <c r="G69" s="42"/>
-      <c r="J69" s="39"/>
-    </row>
-    <row r="70" spans="2:17" ht="15" customHeight="1">
+      <c r="F69" s="42"/>
+      <c r="I69" s="39"/>
+    </row>
+    <row r="70" spans="2:16" ht="15" customHeight="1">
       <c r="B70" s="39"/>
-      <c r="J70" s="39"/>
-    </row>
-    <row r="71" spans="2:17" ht="15" customHeight="1">
+      <c r="I70" s="39"/>
+    </row>
+    <row r="71" spans="2:16" ht="15" customHeight="1">
       <c r="B71" s="39"/>
-      <c r="G71" s="67"/>
-      <c r="H71" s="45"/>
-      <c r="J71" s="39"/>
-    </row>
-    <row r="72" spans="2:17" ht="15" customHeight="1">
+      <c r="F71" s="67"/>
+      <c r="G71" s="45"/>
+      <c r="I71" s="39"/>
+    </row>
+    <row r="72" spans="2:16" ht="15" customHeight="1">
       <c r="B72" s="39"/>
-      <c r="G72" s="42"/>
-      <c r="J72" s="39"/>
-    </row>
-    <row r="73" spans="2:17" ht="15" customHeight="1">
+      <c r="F72" s="42"/>
+      <c r="I72" s="39"/>
+    </row>
+    <row r="73" spans="2:16" ht="15" customHeight="1">
       <c r="B73" s="39"/>
-      <c r="J73" s="39"/>
-    </row>
-    <row r="74" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="I73" s="39"/>
+    </row>
+    <row r="74" spans="2:16" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B74" s="35"/>
       <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="53"/>
-      <c r="F74" s="61"/>
-      <c r="G74" s="51"/>
-      <c r="H74" s="58"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="35"/>
+      <c r="D74" s="53"/>
+      <c r="E74" s="61"/>
+      <c r="F74" s="51"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="38"/>
       <c r="K74" s="38"/>
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
       <c r="N74" s="38"/>
       <c r="O74" s="38"/>
       <c r="P74" s="38"/>
-      <c r="Q74" s="38"/>
-    </row>
-    <row r="75" spans="2:17" ht="15" customHeight="1">
+    </row>
+    <row r="75" spans="2:16" ht="15" customHeight="1">
       <c r="B75" s="35"/>
       <c r="C75" s="51"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="61"/>
-      <c r="G75" s="51"/>
-      <c r="H75" s="58"/>
-      <c r="J75" s="35"/>
-    </row>
-    <row r="76" spans="2:17" ht="15" customHeight="1">
+      <c r="D75" s="53"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="51"/>
+      <c r="G75" s="58"/>
+      <c r="I75" s="35"/>
+    </row>
+    <row r="76" spans="2:16" ht="15" customHeight="1">
       <c r="B76" s="35"/>
       <c r="C76" s="51"/>
       <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="61"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="64"/>
-      <c r="J76" s="35"/>
-    </row>
-    <row r="77" spans="2:17" ht="15" customHeight="1">
+      <c r="E76" s="61"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="64"/>
+      <c r="I76" s="35"/>
+    </row>
+    <row r="77" spans="2:16" ht="15" customHeight="1">
       <c r="B77" s="35"/>
       <c r="C77" s="51"/>
       <c r="D77" s="51"/>
-      <c r="E77" s="51"/>
-      <c r="F77" s="61"/>
-      <c r="G77" s="51"/>
-      <c r="H77" s="64"/>
-      <c r="J77" s="35"/>
-    </row>
-    <row r="78" spans="2:17" ht="15" customHeight="1">
+      <c r="E77" s="61"/>
+      <c r="F77" s="51"/>
+      <c r="G77" s="64"/>
+      <c r="I77" s="35"/>
+    </row>
+    <row r="78" spans="2:16" ht="15" customHeight="1">
       <c r="B78" s="35"/>
       <c r="C78" s="51"/>
       <c r="D78" s="51"/>
-      <c r="E78" s="51"/>
-      <c r="F78" s="61"/>
-      <c r="G78" s="51"/>
-      <c r="H78" s="64"/>
-      <c r="J78" s="35"/>
-    </row>
-    <row r="79" spans="2:17" ht="15" customHeight="1">
+      <c r="E78" s="61"/>
+      <c r="F78" s="51"/>
+      <c r="G78" s="64"/>
+      <c r="I78" s="35"/>
+    </row>
+    <row r="79" spans="2:16" ht="15" customHeight="1">
       <c r="B79" s="35"/>
       <c r="C79" s="51"/>
       <c r="D79" s="51"/>
-      <c r="E79" s="51"/>
-      <c r="F79" s="61"/>
-      <c r="G79" s="51"/>
-      <c r="H79" s="64"/>
-      <c r="J79" s="35"/>
-    </row>
-    <row r="80" spans="2:17" ht="15" customHeight="1">
+      <c r="E79" s="61"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="64"/>
+      <c r="I79" s="35"/>
+    </row>
+    <row r="80" spans="2:16" ht="15" customHeight="1">
       <c r="B80" s="35"/>
       <c r="C80" s="51"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="53"/>
-      <c r="F80" s="61"/>
-      <c r="G80" s="51"/>
-      <c r="H80" s="58"/>
-      <c r="J80" s="35"/>
-    </row>
-    <row r="81" spans="2:18" ht="15" customHeight="1">
+      <c r="D80" s="53"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="51"/>
+      <c r="G80" s="58"/>
+      <c r="I80" s="35"/>
+    </row>
+    <row r="81" spans="2:17" ht="15" customHeight="1">
       <c r="B81" s="35"/>
       <c r="C81" s="51"/>
       <c r="D81" s="51"/>
-      <c r="E81" s="51"/>
-      <c r="F81" s="61"/>
-      <c r="G81" s="51"/>
-      <c r="H81" s="64"/>
-      <c r="J81" s="35"/>
-    </row>
-    <row r="82" spans="2:18" ht="15" customHeight="1">
+      <c r="E81" s="61"/>
+      <c r="F81" s="51"/>
+      <c r="G81" s="64"/>
+      <c r="I81" s="35"/>
+    </row>
+    <row r="82" spans="2:17" ht="15" customHeight="1">
       <c r="B82" s="35"/>
       <c r="C82" s="51"/>
       <c r="D82" s="51"/>
-      <c r="E82" s="51"/>
-      <c r="F82" s="61"/>
-      <c r="G82" s="51"/>
-      <c r="H82" s="64"/>
-      <c r="J82" s="6"/>
-    </row>
-    <row r="83" spans="2:18" s="40" customFormat="1" ht="15" customHeight="1">
+      <c r="E82" s="61"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="64"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="2:17" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="B83" s="35"/>
       <c r="C83" s="51"/>
       <c r="D83" s="51"/>
-      <c r="E83" s="51"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="51"/>
-      <c r="H83" s="63"/>
-      <c r="I83" s="38"/>
-      <c r="J83" s="35"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="51"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="35"/>
+      <c r="J83" s="38"/>
       <c r="K83" s="38"/>
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>
@@ -13047,310 +12923,293 @@
       <c r="O83" s="38"/>
       <c r="P83" s="38"/>
       <c r="Q83" s="38"/>
-      <c r="R83" s="38"/>
-    </row>
-    <row r="84" spans="2:18" ht="15" customHeight="1">
+    </row>
+    <row r="84" spans="2:17" ht="15" customHeight="1">
       <c r="B84" s="35"/>
       <c r="C84" s="51"/>
       <c r="D84" s="51"/>
-      <c r="E84" s="51"/>
-      <c r="F84" s="61"/>
-      <c r="G84" s="51"/>
-      <c r="H84" s="63"/>
-      <c r="J84" s="35"/>
-    </row>
-    <row r="85" spans="2:18" ht="15" customHeight="1">
+      <c r="E84" s="61"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="63"/>
+      <c r="I84" s="35"/>
+    </row>
+    <row r="85" spans="2:17" ht="15" customHeight="1">
       <c r="B85" s="6"/>
       <c r="C85" s="51"/>
-      <c r="D85" s="51"/>
-      <c r="E85" s="53"/>
-      <c r="F85" s="61"/>
-      <c r="G85" s="51"/>
-      <c r="H85" s="58"/>
-      <c r="J85" s="35"/>
-    </row>
-    <row r="86" spans="2:18" ht="15" customHeight="1">
+      <c r="D85" s="53"/>
+      <c r="E85" s="61"/>
+      <c r="F85" s="51"/>
+      <c r="G85" s="58"/>
+      <c r="I85" s="35"/>
+    </row>
+    <row r="86" spans="2:17" ht="15" customHeight="1">
       <c r="B86" s="6"/>
       <c r="C86" s="51"/>
       <c r="D86" s="51"/>
-      <c r="E86" s="51"/>
-      <c r="F86" s="61"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="58"/>
-      <c r="J86" s="35"/>
-    </row>
-    <row r="87" spans="2:18" ht="15" customHeight="1">
+      <c r="E86" s="61"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="58"/>
+      <c r="I86" s="35"/>
+    </row>
+    <row r="87" spans="2:17" ht="15" customHeight="1">
       <c r="B87" s="35"/>
       <c r="C87" s="51"/>
       <c r="D87" s="51"/>
-      <c r="E87" s="51"/>
-      <c r="F87" s="50"/>
-      <c r="G87" s="51"/>
-      <c r="H87" s="59"/>
-      <c r="J87" s="35"/>
-    </row>
-    <row r="88" spans="2:18" ht="15" customHeight="1">
+      <c r="E87" s="50"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="59"/>
+      <c r="I87" s="35"/>
+    </row>
+    <row r="88" spans="2:17" ht="15" customHeight="1">
       <c r="B88" s="6"/>
       <c r="C88" s="51"/>
-      <c r="D88" s="51"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="61"/>
-      <c r="G88" s="51"/>
-      <c r="H88" s="59"/>
-      <c r="J88" s="35"/>
-    </row>
-    <row r="89" spans="2:18" ht="15" customHeight="1">
+      <c r="D88" s="53"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="51"/>
+      <c r="G88" s="59"/>
+      <c r="I88" s="35"/>
+    </row>
+    <row r="89" spans="2:17" ht="15" customHeight="1">
       <c r="B89" s="7"/>
       <c r="C89" s="54"/>
-      <c r="D89" s="54"/>
-      <c r="E89" s="62"/>
-      <c r="F89" s="50"/>
-      <c r="G89" s="61"/>
-      <c r="H89" s="65"/>
-      <c r="J89" s="65"/>
-    </row>
-    <row r="90" spans="2:18" ht="15" customHeight="1">
+      <c r="D89" s="62"/>
+      <c r="E89" s="50"/>
+      <c r="F89" s="61"/>
+      <c r="G89" s="65"/>
+      <c r="I89" s="65"/>
+    </row>
+    <row r="90" spans="2:17" ht="15" customHeight="1">
       <c r="B90" s="52"/>
       <c r="C90" s="48"/>
-      <c r="D90" s="48"/>
-      <c r="E90" s="49"/>
-      <c r="F90" s="55"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="52"/>
-      <c r="J90" s="52"/>
-    </row>
-    <row r="91" spans="2:18" ht="15" customHeight="1">
+      <c r="D90" s="49"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="56"/>
+      <c r="G90" s="52"/>
+      <c r="I90" s="52"/>
+    </row>
+    <row r="91" spans="2:17" ht="15" customHeight="1">
       <c r="B91" s="52"/>
       <c r="C91" s="48"/>
       <c r="D91" s="48"/>
-      <c r="E91" s="48"/>
-      <c r="F91" s="55"/>
-      <c r="G91" s="56"/>
-      <c r="H91" s="52"/>
-      <c r="J91" s="52"/>
-    </row>
-    <row r="92" spans="2:18" ht="15" customHeight="1">
+      <c r="E91" s="55"/>
+      <c r="F91" s="56"/>
+      <c r="G91" s="52"/>
+      <c r="I91" s="52"/>
+    </row>
+    <row r="92" spans="2:17" ht="15" customHeight="1">
       <c r="B92" s="52"/>
       <c r="C92" s="48"/>
       <c r="D92" s="48"/>
-      <c r="E92" s="48"/>
-      <c r="F92" s="55"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="52"/>
-      <c r="J92" s="52"/>
-    </row>
-    <row r="93" spans="2:18" ht="15" customHeight="1">
+      <c r="E92" s="55"/>
+      <c r="F92" s="56"/>
+      <c r="G92" s="52"/>
+      <c r="I92" s="52"/>
+    </row>
+    <row r="93" spans="2:17" ht="15" customHeight="1">
       <c r="B93" s="52"/>
       <c r="C93" s="48"/>
       <c r="D93" s="48"/>
-      <c r="E93" s="48"/>
-      <c r="F93" s="55"/>
-      <c r="G93" s="56"/>
-      <c r="H93" s="52"/>
-      <c r="J93" s="52"/>
-    </row>
-    <row r="94" spans="2:18" ht="15" customHeight="1">
+      <c r="E93" s="55"/>
+      <c r="F93" s="56"/>
+      <c r="G93" s="52"/>
+      <c r="I93" s="52"/>
+    </row>
+    <row r="94" spans="2:17" ht="15" customHeight="1">
       <c r="B94" s="52"/>
       <c r="C94" s="48"/>
       <c r="D94" s="48"/>
-      <c r="E94" s="48"/>
-      <c r="F94" s="55"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="52"/>
-      <c r="J94" s="52"/>
-    </row>
-    <row r="95" spans="2:18" ht="15" customHeight="1">
+      <c r="E94" s="55"/>
+      <c r="F94" s="56"/>
+      <c r="G94" s="52"/>
+      <c r="I94" s="52"/>
+    </row>
+    <row r="95" spans="2:17" ht="15" customHeight="1">
       <c r="B95" s="52"/>
       <c r="C95" s="48"/>
       <c r="D95" s="48"/>
-      <c r="E95" s="48"/>
-      <c r="F95" s="55"/>
-      <c r="G95" s="56"/>
-      <c r="H95" s="52"/>
-      <c r="J95" s="52"/>
-    </row>
-    <row r="96" spans="2:18" ht="15" customHeight="1">
+      <c r="E95" s="55"/>
+      <c r="F95" s="56"/>
+      <c r="G95" s="52"/>
+      <c r="I95" s="52"/>
+    </row>
+    <row r="96" spans="2:17" ht="15" customHeight="1">
       <c r="B96" s="52"/>
       <c r="C96" s="48"/>
       <c r="D96" s="48"/>
-      <c r="E96" s="48"/>
-      <c r="F96" s="55"/>
-      <c r="G96" s="56"/>
-      <c r="H96" s="52"/>
-      <c r="J96" s="52"/>
-    </row>
-    <row r="97" spans="2:10" ht="15" customHeight="1">
+      <c r="E96" s="55"/>
+      <c r="F96" s="56"/>
+      <c r="G96" s="52"/>
+      <c r="I96" s="52"/>
+    </row>
+    <row r="97" spans="2:9" ht="15" customHeight="1">
       <c r="B97" s="52"/>
       <c r="C97" s="48"/>
       <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="55"/>
-      <c r="G97" s="56"/>
-      <c r="H97" s="60"/>
-      <c r="J97" s="52"/>
-    </row>
-    <row r="98" spans="2:10" ht="15" customHeight="1">
+      <c r="E97" s="55"/>
+      <c r="F97" s="56"/>
+      <c r="G97" s="60"/>
+      <c r="I97" s="52"/>
+    </row>
+    <row r="98" spans="2:9" ht="15" customHeight="1">
       <c r="B98" s="52"/>
       <c r="C98" s="48"/>
       <c r="D98" s="48"/>
-      <c r="E98" s="48"/>
-      <c r="F98" s="55"/>
-      <c r="G98" s="57"/>
-      <c r="H98" s="60"/>
-      <c r="J98" s="52"/>
-    </row>
-    <row r="99" spans="2:10" ht="15" customHeight="1">
+      <c r="E98" s="55"/>
+      <c r="F98" s="57"/>
+      <c r="G98" s="60"/>
+      <c r="I98" s="52"/>
+    </row>
+    <row r="99" spans="2:9" ht="15" customHeight="1">
       <c r="B99" s="39"/>
-      <c r="G99" s="42"/>
-      <c r="H99" s="39"/>
-    </row>
-    <row r="100" spans="2:10" ht="15" customHeight="1">
+      <c r="F99" s="42"/>
+      <c r="G99" s="39"/>
+    </row>
+    <row r="100" spans="2:9" ht="15" customHeight="1">
       <c r="B100" s="39"/>
-      <c r="H100" s="39"/>
-    </row>
-    <row r="101" spans="2:10" ht="15" customHeight="1">
+      <c r="G100" s="39"/>
+    </row>
+    <row r="101" spans="2:9" ht="15" customHeight="1">
       <c r="B101" s="39"/>
-      <c r="H101" s="39"/>
-    </row>
-    <row r="102" spans="2:10" ht="15" customHeight="1">
+      <c r="G101" s="39"/>
+    </row>
+    <row r="102" spans="2:9" ht="15" customHeight="1">
       <c r="B102" s="39"/>
-      <c r="H102" s="39"/>
-      <c r="I102" s="45"/>
-    </row>
-    <row r="103" spans="2:10" ht="15" customHeight="1">
+      <c r="G102" s="39"/>
+      <c r="H102" s="45"/>
+    </row>
+    <row r="103" spans="2:9" ht="15" customHeight="1">
       <c r="B103" s="39"/>
-      <c r="G103" s="42"/>
-      <c r="H103" s="39"/>
-    </row>
-    <row r="104" spans="2:10" ht="15" customHeight="1">
+      <c r="F103" s="42"/>
+      <c r="G103" s="39"/>
+    </row>
+    <row r="104" spans="2:9" ht="15" customHeight="1">
       <c r="B104" s="39"/>
-      <c r="H104" s="39"/>
-    </row>
-    <row r="105" spans="2:10" ht="15" customHeight="1">
+      <c r="G104" s="39"/>
+    </row>
+    <row r="105" spans="2:9" ht="15" customHeight="1">
       <c r="B105" s="39"/>
-      <c r="G105" s="42"/>
-      <c r="H105" s="39"/>
-    </row>
-    <row r="106" spans="2:10" ht="15" customHeight="1">
+      <c r="F105" s="42"/>
+      <c r="G105" s="39"/>
+    </row>
+    <row r="106" spans="2:9" ht="15" customHeight="1">
       <c r="B106" s="39"/>
-      <c r="G106" s="42"/>
-      <c r="H106" s="39"/>
-    </row>
-    <row r="107" spans="2:10" ht="15" customHeight="1">
+      <c r="F106" s="42"/>
+      <c r="G106" s="39"/>
+    </row>
+    <row r="107" spans="2:9" ht="15" customHeight="1">
       <c r="B107" s="39"/>
-      <c r="H107" s="39"/>
-    </row>
-    <row r="108" spans="2:10" ht="15" customHeight="1">
+      <c r="G107" s="39"/>
+    </row>
+    <row r="108" spans="2:9" ht="15" customHeight="1">
       <c r="B108" s="39"/>
-      <c r="H108" s="39"/>
-    </row>
-    <row r="109" spans="2:10" ht="15" customHeight="1">
+      <c r="G108" s="39"/>
+    </row>
+    <row r="109" spans="2:9" ht="15" customHeight="1">
       <c r="B109" s="39"/>
-      <c r="H109" s="39"/>
-    </row>
-    <row r="110" spans="2:10" ht="15" customHeight="1">
+      <c r="G109" s="39"/>
+    </row>
+    <row r="110" spans="2:9" ht="15" customHeight="1">
       <c r="B110" s="39"/>
-      <c r="H110" s="39"/>
-    </row>
-    <row r="111" spans="2:10" ht="15" customHeight="1">
+      <c r="G110" s="39"/>
+    </row>
+    <row r="111" spans="2:9" ht="15" customHeight="1">
       <c r="B111" s="39"/>
-      <c r="H111" s="39"/>
-    </row>
-    <row r="112" spans="2:10" ht="15" customHeight="1">
+      <c r="G111" s="39"/>
+    </row>
+    <row r="112" spans="2:9" ht="15" customHeight="1">
       <c r="B112" s="39"/>
-      <c r="H112" s="39"/>
-    </row>
-    <row r="113" spans="2:8" ht="15" customHeight="1">
+      <c r="G112" s="39"/>
+    </row>
+    <row r="113" spans="2:7" ht="15" customHeight="1">
       <c r="B113" s="39"/>
-      <c r="H113" s="39"/>
-    </row>
-    <row r="114" spans="2:8" ht="15" customHeight="1">
+      <c r="G113" s="39"/>
+    </row>
+    <row r="114" spans="2:7" ht="15" customHeight="1">
       <c r="B114" s="39"/>
-      <c r="H114" s="39"/>
-    </row>
-    <row r="115" spans="2:8" ht="15" customHeight="1">
+      <c r="G114" s="39"/>
+    </row>
+    <row r="115" spans="2:7" ht="15" customHeight="1">
       <c r="B115" s="39"/>
-      <c r="H115" s="39"/>
-    </row>
-    <row r="116" spans="2:8" ht="15" customHeight="1">
+      <c r="G115" s="39"/>
+    </row>
+    <row r="116" spans="2:7" ht="15" customHeight="1">
       <c r="B116" s="39"/>
-      <c r="H116" s="39"/>
-    </row>
-    <row r="117" spans="2:8" ht="15" customHeight="1">
+      <c r="G116" s="39"/>
+    </row>
+    <row r="117" spans="2:7" ht="15" customHeight="1">
       <c r="B117" s="39"/>
-      <c r="G117" s="42"/>
-      <c r="H117" s="39"/>
-    </row>
-    <row r="118" spans="2:8" ht="15" customHeight="1">
+      <c r="F117" s="42"/>
+      <c r="G117" s="39"/>
+    </row>
+    <row r="118" spans="2:7" ht="15" customHeight="1">
       <c r="B118" s="39"/>
-      <c r="H118" s="39"/>
-    </row>
-    <row r="119" spans="2:8" ht="15" customHeight="1">
+      <c r="G118" s="39"/>
+    </row>
+    <row r="119" spans="2:7" ht="15" customHeight="1">
       <c r="B119" s="39"/>
-      <c r="G119" s="42"/>
-      <c r="H119" s="39"/>
-    </row>
-    <row r="120" spans="2:8" ht="15" customHeight="1">
+      <c r="F119" s="42"/>
+      <c r="G119" s="39"/>
+    </row>
+    <row r="120" spans="2:7" ht="15" customHeight="1">
       <c r="B120" s="39"/>
-      <c r="H120" s="39"/>
-    </row>
-    <row r="121" spans="2:8" ht="15" customHeight="1">
+      <c r="G120" s="39"/>
+    </row>
+    <row r="121" spans="2:7" ht="15" customHeight="1">
       <c r="B121" s="39"/>
-      <c r="G121" s="42"/>
-      <c r="H121" s="39"/>
-    </row>
-    <row r="122" spans="2:8" ht="15" customHeight="1">
+      <c r="F121" s="42"/>
+      <c r="G121" s="39"/>
+    </row>
+    <row r="122" spans="2:7" ht="15" customHeight="1">
       <c r="B122" s="39"/>
-      <c r="H122" s="39"/>
-    </row>
-    <row r="123" spans="2:8" ht="15" customHeight="1">
+      <c r="G122" s="39"/>
+    </row>
+    <row r="123" spans="2:7" ht="15" customHeight="1">
       <c r="B123" s="39"/>
-      <c r="G123" s="42"/>
-      <c r="H123" s="39"/>
-    </row>
-    <row r="124" spans="2:8" ht="15" customHeight="1">
+      <c r="F123" s="42"/>
+      <c r="G123" s="39"/>
+    </row>
+    <row r="124" spans="2:7" ht="15" customHeight="1">
       <c r="B124" s="39"/>
-      <c r="H124" s="39"/>
-    </row>
-    <row r="125" spans="2:8" ht="15" customHeight="1">
+      <c r="G124" s="39"/>
+    </row>
+    <row r="125" spans="2:7" ht="15" customHeight="1">
       <c r="B125" s="39"/>
-      <c r="H125" s="39"/>
-    </row>
-    <row r="126" spans="2:8" ht="15" customHeight="1">
+      <c r="G125" s="39"/>
+    </row>
+    <row r="126" spans="2:7" ht="15" customHeight="1">
       <c r="B126" s="36"/>
       <c r="C126" s="37"/>
       <c r="D126" s="37"/>
-      <c r="E126" s="37"/>
-      <c r="H126" s="36"/>
-    </row>
-    <row r="127" spans="2:8" ht="15" customHeight="1">
+      <c r="G126" s="36"/>
+    </row>
+    <row r="127" spans="2:7" ht="15" customHeight="1">
       <c r="B127" s="39"/>
-      <c r="G127" s="42"/>
-      <c r="H127" s="39"/>
-    </row>
-    <row r="143" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F143" s="51"/>
-    </row>
-    <row r="144" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F144" s="51"/>
-    </row>
-    <row r="145" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F145" s="51"/>
-    </row>
-    <row r="146" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F146" s="51"/>
-    </row>
-    <row r="147" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F147" s="51"/>
-    </row>
-    <row r="148" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F148" s="51"/>
-    </row>
-    <row r="149" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F149" s="51"/>
-    </row>
-    <row r="150" spans="6:6" s="35" customFormat="1" ht="15" customHeight="1">
-      <c r="F150" s="51"/>
+      <c r="F127" s="42"/>
+      <c r="G127" s="39"/>
+    </row>
+    <row r="143" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E143" s="51"/>
+    </row>
+    <row r="144" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E144" s="51"/>
+    </row>
+    <row r="145" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E145" s="51"/>
+    </row>
+    <row r="146" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E146" s="51"/>
+    </row>
+    <row r="147" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E147" s="51"/>
+    </row>
+    <row r="148" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E148" s="51"/>
+    </row>
+    <row r="149" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E149" s="51"/>
+    </row>
+    <row r="150" spans="5:5" s="35" customFormat="1" ht="15" customHeight="1">
+      <c r="E150" s="51"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -13366,257 +13225,249 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A40:M46"/>
+  <dimension ref="A40:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="40" spans="1:13" ht="15.75">
-      <c r="A40" s="74" t="s">
+    <row r="40" spans="1:12" ht="15.75">
+      <c r="A40" s="76" t="s">
         <v>345</v>
       </c>
       <c r="B40" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="76" t="s">
+      <c r="D40" s="78" t="s">
         <v>358</v>
       </c>
-      <c r="E40" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="F40" s="75" t="s">
+      <c r="E40" s="77" t="s">
         <v>333</v>
       </c>
+      <c r="F40" s="77" t="s">
+        <v>334</v>
+      </c>
       <c r="G40" s="77" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H40" s="77" t="s">
-        <v>335</v>
-      </c>
-      <c r="I40" s="79" t="s">
         <v>336</v>
       </c>
-      <c r="J40" s="77" t="s">
+      <c r="I40" s="77" t="s">
         <v>337</v>
       </c>
-      <c r="K40" s="74" t="s">
+      <c r="J40" s="76" t="s">
         <v>359</v>
       </c>
-      <c r="L40" s="74" t="s">
+      <c r="K40" s="76" t="s">
         <v>343</v>
       </c>
-      <c r="M40" s="74" t="s">
+      <c r="L40" s="76" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:12">
       <c r="A41" s="16"/>
       <c r="B41" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="D41" s="69"/>
-      <c r="E41" s="70" t="s">
+      <c r="D41" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="F41" s="70" t="s">
+      <c r="E41" s="69" t="s">
         <v>326</v>
       </c>
-      <c r="G41" s="70" t="s">
+      <c r="F41" s="69" t="s">
         <v>327</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="G41" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="I41" s="16"/>
-      <c r="J41" s="19" t="s">
+      <c r="H41" s="16"/>
+      <c r="I41" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="K41" s="17" t="s">
+      <c r="J41" s="17" t="s">
         <v>346</v>
       </c>
+      <c r="K41" s="17"/>
       <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-    </row>
-    <row r="42" spans="1:13">
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="16"/>
       <c r="B42" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="C42" s="70">
+      <c r="C42" s="69">
         <v>9</v>
       </c>
       <c r="D42" s="69"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70" t="s">
+      <c r="E42" s="69" t="s">
         <v>331</v>
       </c>
-      <c r="G42" s="70" t="s">
+      <c r="F42" s="69" t="s">
         <v>327</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="G42" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="19" t="s">
+      <c r="H42" s="16"/>
+      <c r="I42" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="K42" s="17" t="s">
+      <c r="J42" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="L42" s="17">
+      <c r="K42" s="17">
         <v>11223</v>
       </c>
-      <c r="M42" s="17"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="L42" s="17"/>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="16"/>
       <c r="B43" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="69" t="s">
         <v>264</v>
       </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="70" t="s">
+      <c r="D43" s="69" t="s">
         <v>341</v>
       </c>
+      <c r="E43" s="69" t="s">
+        <v>326</v>
+      </c>
       <c r="F43" s="70" t="s">
-        <v>326</v>
-      </c>
-      <c r="G43" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="G43" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="19" t="s">
+      <c r="H43" s="16"/>
+      <c r="I43" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="J43" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17" t="s">
+      <c r="K43" s="17"/>
+      <c r="L43" s="17" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:12">
       <c r="A44" s="16"/>
       <c r="B44" s="19" t="s">
         <v>357</v>
       </c>
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="69"/>
-      <c r="E44" s="70" t="s">
+      <c r="D44" s="69" t="s">
         <v>340</v>
       </c>
-      <c r="F44" s="70" t="s">
+      <c r="E44" s="69" t="s">
         <v>326</v>
       </c>
-      <c r="G44" s="70" t="s">
+      <c r="F44" s="69" t="s">
         <v>329</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="G44" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="I44" s="16"/>
-      <c r="J44" s="19" t="s">
+      <c r="H44" s="16"/>
+      <c r="I44" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="K44" s="17" t="s">
+      <c r="J44" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="L44" s="17">
+      <c r="K44" s="17">
         <v>987807</v>
       </c>
-      <c r="M44" s="17" t="s">
+      <c r="L44" s="17" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:12">
       <c r="A45" s="16"/>
       <c r="B45" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="70" t="s">
+      <c r="D45" s="69" t="s">
         <v>342</v>
       </c>
-      <c r="F45" s="70" t="s">
+      <c r="E45" s="69" t="s">
         <v>326</v>
       </c>
+      <c r="F45" s="71" t="s">
+        <v>327</v>
+      </c>
       <c r="G45" s="72" t="s">
-        <v>327</v>
-      </c>
-      <c r="H45" s="73" t="s">
         <v>330</v>
       </c>
-      <c r="I45" s="16"/>
-      <c r="J45" s="19" t="s">
+      <c r="H45" s="16"/>
+      <c r="I45" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="J45" s="17" t="s">
         <v>346</v>
       </c>
+      <c r="K45" s="17"/>
       <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-    </row>
-    <row r="46" spans="1:13">
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="16"/>
       <c r="B46" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="C46" s="70">
+      <c r="C46" s="69">
         <v>7</v>
       </c>
       <c r="D46" s="69"/>
-      <c r="E46" s="70"/>
+      <c r="E46" s="69" t="s">
+        <v>331</v>
+      </c>
       <c r="F46" s="70" t="s">
-        <v>331</v>
-      </c>
-      <c r="G46" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="G46" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="I46" s="16"/>
-      <c r="J46" s="19" t="s">
+      <c r="H46" s="16"/>
+      <c r="I46" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="K46" s="17" t="s">
+      <c r="J46" s="17" t="s">
         <v>350</v>
       </c>
+      <c r="K46" s="17"/>
       <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>